<commit_message>
cellpose multisess by registering against first session data_avg, then avg over cellpose_tiff of each sess
</commit_message>
<xml_diff>
--- a/data/adp_dataset_master.xlsx
+++ b/data/adp_dataset_master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9759359C-F8F4-451E-AD60-30A2199EA324}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE06493-855B-4766-A2E7-E17169669627}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="14380" windowHeight="4150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="14376" windowHeight="4152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="42">
   <si>
     <t>mouse</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>cellpose_seg</t>
+  </si>
+  <si>
+    <t>mix50 high res. vis deg 20</t>
+  </si>
+  <si>
+    <t>mix50 high res. vis deg 30</t>
+  </si>
+  <si>
+    <t>only 1 ori grating</t>
   </si>
 </sst>
 </file>
@@ -590,29 +599,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93:B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,12 +653,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B2" s="1">
-        <v>200803</v>
+        <v>200720</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -658,7 +667,7 @@
         <v>200</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="b">
         <v>1</v>
@@ -669,13 +678,16 @@
       <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B3" s="1">
-        <v>200804</v>
+        <v>200721</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -696,12 +708,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B4" s="1">
-        <v>200806</v>
+        <v>200723</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -722,12 +734,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B5" s="1">
-        <v>200720</v>
+        <v>200728</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -747,16 +759,13 @@
       <c r="I5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B6" s="1">
-        <v>200721</v>
+        <v>200729</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -777,18 +786,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B7" s="1">
-        <v>200723</v>
+        <v>200803</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>200</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
@@ -799,25 +811,19 @@
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B8" s="1">
-        <v>200728</v>
+        <v>200804</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>200</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
@@ -828,16 +834,19 @@
       <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B9" s="1">
-        <v>200729</v>
+        <v>200806</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
         <v>200</v>
@@ -855,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1328</v>
       </c>
@@ -884,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1328</v>
       </c>
@@ -913,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1328</v>
       </c>
@@ -942,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1328</v>
       </c>
@@ -971,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1328</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1329</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1329</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1329</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1329</v>
       </c>
@@ -1093,7 +1102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1329</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1337</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1337</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1337</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1337</v>
       </c>
@@ -1211,7 +1220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1337</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1337</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1338</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1338</v>
       </c>
@@ -1303,86 +1312,82 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>1338</v>
-      </c>
-      <c r="B28" s="2">
-        <v>210616</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2">
-        <v>200</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2" t="s">
-        <v>35</v>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B28" s="1">
+        <v>210401</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>150</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>1338</v>
-      </c>
-      <c r="B29" s="9">
-        <v>210805</v>
+        <v>33303</v>
+      </c>
+      <c r="B29" s="1">
+        <v>210405</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
         <v>150</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>1339</v>
+        <v>33303</v>
       </c>
       <c r="B30" s="1">
-        <v>210908</v>
+        <v>210415</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
         <v>150</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>1339</v>
+        <v>33303</v>
       </c>
       <c r="B31" s="1">
-        <v>210922</v>
+        <v>210415</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
@@ -1391,597 +1396,604 @@
         <v>200</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="1" t="b">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B32" s="1">
+        <v>210419</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>200</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B33" s="2">
+        <v>210419</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>150</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B34" s="2">
+        <v>210422</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>200</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B35" s="2">
+        <v>210422</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>150</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B36" s="2">
+        <v>210430</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>200</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="H36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B37" s="2">
+        <v>210430</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>150</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="H37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B38" s="2">
+        <v>210506</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>200</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B39" s="2">
+        <v>210603</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>150</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>33303</v>
+      </c>
+      <c r="B40" s="2">
+        <v>210610</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>150</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="H40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>1338</v>
+      </c>
+      <c r="B41" s="2">
+        <v>210616</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="2">
+        <v>200</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>1339</v>
-      </c>
-      <c r="B32" s="1">
-        <v>210922</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>200</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>1339</v>
-      </c>
-      <c r="B33" s="1">
-        <v>210922</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1">
-        <v>200</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>1339</v>
-      </c>
-      <c r="B34" s="1">
-        <v>210930</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="1">
-        <v>200</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>1339</v>
-      </c>
-      <c r="B35" s="1">
-        <v>210930</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="1">
-        <v>150</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>1350</v>
-      </c>
-      <c r="B36" s="1">
-        <v>211020</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1">
-        <v>200</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>1350</v>
-      </c>
-      <c r="B37" s="1">
-        <v>211020</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="1">
-        <v>150</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>1350</v>
-      </c>
-      <c r="B38" s="1">
-        <v>211028</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="1">
-        <v>200</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>1350</v>
-      </c>
-      <c r="B39" s="1">
-        <v>211028</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="1">
-        <v>150</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B40" s="2">
-        <v>211222</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="2">
-        <v>200</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B41" s="2">
-        <v>211222</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="2">
-        <v>200</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="7"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B42" s="2">
-        <v>211222</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="2">
-        <v>200</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2" t="s">
-        <v>32</v>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B42" s="1">
+        <v>210617</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1">
+        <v>150</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B43" s="2">
-        <v>220124</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>33303</v>
+      </c>
+      <c r="B43" s="1">
+        <v>210623</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>150</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>1338</v>
+      </c>
+      <c r="B44" s="9">
+        <v>210805</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="2">
-        <v>200</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B44" s="2">
-        <v>220124</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="1">
+        <v>150</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B45" s="1">
+        <v>210908</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="2">
-        <v>200</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B45" s="2">
-        <v>220225</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="2">
-        <v>200</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="1" t="b">
+      <c r="D45" s="1">
+        <v>150</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B46" s="1">
+        <v>210922</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
+        <v>200</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
-        <v>1350</v>
-      </c>
-      <c r="B46" s="2">
-        <v>220225</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="2">
-        <v>200</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="7"/>
-      <c r="H46" s="2" t="s">
-        <v>33</v>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>1351</v>
+        <v>1339</v>
       </c>
       <c r="B47" s="1">
-        <v>220228</v>
+        <v>210922</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1">
         <v>200</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>1351</v>
+        <v>1339</v>
       </c>
       <c r="B48" s="1">
-        <v>220228</v>
+        <v>210922</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
-        <v>1369</v>
-      </c>
-      <c r="B49" s="2">
-        <v>220310</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="2">
-        <v>200</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>33</v>
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B49" s="1">
+        <v>210930</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1">
+        <v>200</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
-        <v>1369</v>
-      </c>
-      <c r="B50" s="2">
-        <v>220310</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="2">
-        <v>200</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="H50" s="2" t="s">
-        <v>33</v>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>1339</v>
+      </c>
+      <c r="B50" s="1">
+        <v>210930</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1">
+        <v>150</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
-        <v>1369</v>
-      </c>
-      <c r="B51" s="2">
-        <v>220311</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>44405</v>
+      </c>
+      <c r="B51" s="1">
+        <v>211011</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
+        <v>200</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>44405</v>
+      </c>
+      <c r="B52" s="1">
+        <v>211011</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>200</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>44405</v>
+      </c>
+      <c r="B53" s="1">
+        <v>211011</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1">
+        <v>200</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>1350</v>
+      </c>
+      <c r="B54" s="1">
+        <v>211020</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="2">
-        <v>200</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="7"/>
-      <c r="H51" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
-        <v>1369</v>
-      </c>
-      <c r="B52" s="2">
-        <v>220311</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D54" s="1">
+        <v>200</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>1350</v>
+      </c>
+      <c r="B55" s="1">
+        <v>211020</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D52" s="2">
-        <v>200</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="7"/>
-      <c r="H52" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
-        <v>1372</v>
-      </c>
-      <c r="B53" s="1">
-        <v>220406</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1">
-        <v>200</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
-        <v>1372</v>
-      </c>
-      <c r="B54" s="1">
-        <v>220406</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="1">
-        <v>200</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B55" s="1">
-        <v>210401</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="D55" s="1">
         <v>150</v>
@@ -1990,30 +2002,30 @@
         <v>12</v>
       </c>
       <c r="F55" s="4"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B56" s="1">
-        <v>210405</v>
+        <v>211028</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D56" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="1"/>
@@ -2021,25 +2033,25 @@
         <v>18</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B57" s="1">
-        <v>210415</v>
+        <v>211028</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D57" s="1">
         <v>150</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="1"/>
@@ -2047,272 +2059,277 @@
         <v>18</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B58" s="1">
-        <v>210415</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1">
-        <v>200</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>18</v>
+    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B58" s="2">
+        <v>211222</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="2">
+        <v>200</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
-        <v>33303</v>
-      </c>
-      <c r="B59" s="1">
-        <v>210419</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1">
-        <v>200</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>1350</v>
+      </c>
+      <c r="B59" s="2">
+        <v>211222</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="2">
+        <v>200</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="H59" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B60" s="2">
-        <v>210419</v>
+        <v>211222</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D60" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F60" s="7"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1" t="s">
-        <v>18</v>
+      <c r="H60" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2">
-        <v>33303</v>
-      </c>
-      <c r="B61" s="2">
-        <v>210422</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="2">
-        <v>200</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="7"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B61" s="1">
+        <v>211223</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1">
+        <v>200</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="4"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
-        <v>33303</v>
-      </c>
-      <c r="B62" s="2">
-        <v>210422</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="2">
-        <v>150</v>
-      </c>
-      <c r="E62" s="7" t="s">
+    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B62" s="1">
+        <v>211223</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="1">
+        <v>200</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="7"/>
+      <c r="F62" s="4"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A63" s="2">
-        <v>33303</v>
-      </c>
-      <c r="B63" s="2">
-        <v>210430</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="2">
-        <v>200</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="7"/>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B63" s="1">
+        <v>211223</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1">
+        <v>200</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="H63" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B64" s="2">
-        <v>210430</v>
+        <v>220124</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F64" s="7"/>
-      <c r="H64" s="1" t="s">
-        <v>18</v>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B65" s="2">
-        <v>210506</v>
+        <v>220124</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D65" s="2">
         <v>200</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F65" s="7"/>
-      <c r="H65" s="1" t="s">
-        <v>18</v>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B66" s="2">
-        <v>210603</v>
+        <v>220225</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="H66" s="1" t="s">
-        <v>18</v>
+      <c r="F66" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>33303</v>
+        <v>1350</v>
       </c>
       <c r="B67" s="2">
-        <v>210610</v>
+        <v>220225</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D67" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F67" s="7"/>
-      <c r="H67" s="1" t="s">
-        <v>18</v>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>33303</v>
+        <v>1351</v>
       </c>
       <c r="B68" s="1">
-        <v>210617</v>
+        <v>220228</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>11</v>
@@ -2321,18 +2338,18 @@
         <v>18</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>33303</v>
+        <v>1351</v>
       </c>
       <c r="B69" s="1">
-        <v>210623</v>
+        <v>220228</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D69" s="1">
         <v>150</v>
@@ -2341,203 +2358,221 @@
         <v>11</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A70" s="1">
-        <v>44405</v>
-      </c>
-      <c r="B70" s="1">
-        <v>211011</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D70" s="1">
-        <v>200</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>1369</v>
+      </c>
+      <c r="B70" s="2">
+        <v>220310</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="2">
+        <v>200</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A71" s="1">
-        <v>44405</v>
-      </c>
-      <c r="B71" s="1">
-        <v>211011</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="1">
-        <v>200</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>1369</v>
+      </c>
+      <c r="B71" s="2">
+        <v>220310</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="2">
+        <v>200</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A72" s="1">
-        <v>44405</v>
-      </c>
-      <c r="B72" s="1">
-        <v>211011</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="1">
-        <v>200</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>1369</v>
+      </c>
+      <c r="B72" s="2">
+        <v>220311</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="2">
+        <v>200</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="1">
-        <v>44409</v>
-      </c>
-      <c r="B73" s="1">
-        <v>211223</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D73" s="1">
-        <v>200</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>1369</v>
+      </c>
+      <c r="B73" s="2">
+        <v>220311</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="2">
+        <v>200</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" s="1">
-        <v>44409</v>
-      </c>
-      <c r="B74" s="1">
-        <v>211223</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="1">
-        <v>200</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>44415</v>
+      </c>
+      <c r="B74" s="2">
+        <v>220318</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="2">
+        <v>200</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="7"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="1">
-        <v>44409</v>
-      </c>
-      <c r="B75" s="1">
-        <v>211223</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="1">
-        <v>200</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>32</v>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>44415</v>
+      </c>
+      <c r="B75" s="2">
+        <v>220318</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="2">
+        <v>200</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="2">
-        <v>44415</v>
-      </c>
-      <c r="B76" s="2">
-        <v>220318</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="2">
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B76" s="1">
+        <v>220406</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1">
         <v>200</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F76" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="H76" s="2" t="s">
         <v>34</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="2">
-        <v>44415</v>
-      </c>
-      <c r="B77" s="2">
-        <v>220318</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D77" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B77" s="1">
+        <v>220406</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1">
         <v>200</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F77" s="7"/>
-      <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
         <v>34</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44416</v>
       </c>
@@ -2561,7 +2596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44416</v>
       </c>
@@ -2585,9 +2620,331 @@
         <v>23</v>
       </c>
     </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B80" s="1">
+        <v>220704</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="1">
+        <v>200</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B81" s="1">
+        <v>220704</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1">
+        <v>200</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B82" s="1">
+        <v>220704</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1">
+        <v>200</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B83" s="1">
+        <v>220708</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="1">
+        <v>200</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B84" s="1">
+        <v>220711</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>200</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B85" s="1">
+        <v>220711</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1">
+        <v>200</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B86" s="1">
+        <v>220714</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="1">
+        <v>200</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>1372</v>
+      </c>
+      <c r="B87" s="1">
+        <v>220714</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="1">
+        <v>200</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>1374</v>
+      </c>
+      <c r="B88" s="1">
+        <v>220907</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1">
+        <v>150</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>1374</v>
+      </c>
+      <c r="B89" s="1">
+        <v>220907</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="1">
+        <v>150</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>1374</v>
+      </c>
+      <c r="B90" s="1">
+        <v>220907</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1">
+        <v>150</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>1373</v>
+      </c>
+      <c r="B91" s="1">
+        <v>220909</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1">
+        <v>150</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>1373</v>
+      </c>
+      <c r="B92" s="1">
+        <v>220909</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1">
+        <v>150</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>1373</v>
+      </c>
+      <c r="B93" s="1">
+        <v>220909</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1">
+        <v>150</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J79">
-    <sortCondition ref="A2:A79"/>
+    <sortCondition ref="B2:B79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2602,24 +2959,24 @@
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.08984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.90625" style="1"/>
+    <col min="11" max="11" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2657,7 +3014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1322</v>
       </c>
@@ -2692,7 +3049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1322</v>
       </c>
@@ -2721,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1322</v>
       </c>
@@ -2750,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1323</v>
       </c>
@@ -2785,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1323</v>
       </c>
@@ -2814,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1323</v>
       </c>
@@ -2843,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1324</v>
       </c>
@@ -2878,7 +3235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1324</v>
       </c>
@@ -2907,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1324</v>
       </c>
@@ -2934,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1328</v>
       </c>
@@ -2963,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1328</v>
       </c>
@@ -2992,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1328</v>
       </c>
@@ -3021,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1328</v>
       </c>
@@ -3050,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1328</v>
       </c>
@@ -3080,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1329</v>
       </c>
@@ -3112,7 +3469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1329</v>
       </c>
@@ -3135,7 +3492,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1329</v>
       </c>
@@ -3158,7 +3515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1329</v>
       </c>
@@ -3181,7 +3538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1329</v>
       </c>
@@ -3204,7 +3561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1337</v>
       </c>
@@ -3233,7 +3590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1337</v>
       </c>
@@ -3259,7 +3616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1337</v>
       </c>
@@ -3282,7 +3639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1337</v>
       </c>
@@ -3305,7 +3662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1337</v>
       </c>
@@ -3328,7 +3685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1337</v>
       </c>
@@ -3351,7 +3708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1338</v>
       </c>
@@ -3377,7 +3734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1338</v>
       </c>
@@ -3403,7 +3760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1338</v>
       </c>
@@ -3426,7 +3783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1338</v>
       </c>
@@ -3449,7 +3806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>1338</v>
       </c>
@@ -3479,7 +3836,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>1338</v>
       </c>
@@ -3509,7 +3866,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1338</v>
       </c>
@@ -3539,7 +3896,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>1338</v>
       </c>
@@ -3562,7 +3919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1339</v>
       </c>
@@ -3586,7 +3943,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1339</v>
       </c>
@@ -3610,7 +3967,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1339</v>
       </c>
@@ -3634,7 +3991,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>1339</v>
       </c>
@@ -3658,7 +4015,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>1339</v>
       </c>
@@ -3682,7 +4039,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1339</v>
       </c>
@@ -3706,7 +4063,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1350</v>
       </c>
@@ -3730,7 +4087,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>1350</v>
       </c>
@@ -3754,7 +4111,7 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1350</v>
       </c>
@@ -3778,7 +4135,7 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>1350</v>
       </c>
@@ -3802,7 +4159,7 @@
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>1350</v>
       </c>
@@ -3830,7 +4187,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>1350</v>
       </c>
@@ -3858,7 +4215,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>1350</v>
       </c>
@@ -3886,7 +4243,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>1350</v>
       </c>
@@ -3914,7 +4271,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>1350</v>
       </c>
@@ -3942,7 +4299,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>1350</v>
       </c>
@@ -3965,7 +4322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>1350</v>
       </c>
@@ -3988,7 +4345,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1351</v>
       </c>
@@ -4016,7 +4373,7 @@
       <c r="K52"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>1351</v>
       </c>
@@ -4044,7 +4401,7 @@
       <c r="K53"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>1369</v>
       </c>
@@ -4067,7 +4424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>1369</v>
       </c>
@@ -4090,7 +4447,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>1369</v>
       </c>
@@ -4113,7 +4470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>1369</v>
       </c>
@@ -4136,7 +4493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>1372</v>
       </c>
@@ -4164,7 +4521,7 @@
       <c r="K58"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>1372</v>
       </c>
@@ -4192,7 +4549,7 @@
       <c r="K59"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>33303</v>
       </c>
@@ -4220,7 +4577,7 @@
       <c r="K60"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>33303</v>
       </c>
@@ -4248,7 +4605,7 @@
       <c r="K61"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>33303</v>
       </c>
@@ -4276,7 +4633,7 @@
       <c r="K62"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>33303</v>
       </c>
@@ -4304,7 +4661,7 @@
       <c r="K63"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>33303</v>
       </c>
@@ -4332,7 +4689,7 @@
       <c r="K64"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>33303</v>
       </c>
@@ -4362,7 +4719,7 @@
       <c r="K65"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>33303</v>
       </c>
@@ -4390,7 +4747,7 @@
       <c r="K66"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>33303</v>
       </c>
@@ -4422,7 +4779,7 @@
       <c r="K67"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>33303</v>
       </c>
@@ -4445,7 +4802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>33303</v>
       </c>
@@ -4471,7 +4828,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>33303</v>
       </c>
@@ -4497,7 +4854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>33303</v>
       </c>
@@ -4523,7 +4880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>33303</v>
       </c>
@@ -4549,7 +4906,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>33303</v>
       </c>
@@ -4572,7 +4929,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>33303</v>
       </c>
@@ -4595,7 +4952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>44405</v>
       </c>
@@ -4618,7 +4975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>44405</v>
       </c>
@@ -4641,7 +4998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>44405</v>
       </c>
@@ -4664,7 +5021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44409</v>
       </c>
@@ -4687,7 +5044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44409</v>
       </c>
@@ -4710,7 +5067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>44409</v>
       </c>
@@ -4733,7 +5090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>44415</v>
       </c>
@@ -4761,7 +5118,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>44415</v>
       </c>
@@ -4789,7 +5146,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>44416</v>
       </c>
@@ -4812,7 +5169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>44416</v>
       </c>

</xml_diff>